<commit_message>
Luban Example - Update
- Remove Luban GUI and Odin Inspector
- Use process to execute export task
- Introduce Luban Helper
</commit_message>
<xml_diff>
--- a/samples/LubanExample/Data/Data/__tables__.xlsx
+++ b/samples/LubanExample/Data/Data/__tables__.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20616" windowHeight="9275"/>
+    <workbookView windowWidth="21120" windowHeight="10092"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" fullCalcOnLoad="1" fullPrecision="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -26,79 +26,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>mrhua</author>
-  </authors>
-  <commentList>
-    <comment ref="C4" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <rFont val="宋体"/>
-            <charset val="134"/>
-          </rPr>
-          <t>这个名称将会成为代码中的类名</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E4" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <rFont val="宋体"/>
-            <charset val="134"/>
-          </rPr>
-          <t>使用 子表名@表格文件名 来指定子表
-不指定子表时，将会读取所有格式正确的子表，并合为一个</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G4" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <rFont val="宋体"/>
-            <charset val="134"/>
-          </rPr>
-          <t>默认为map，一般用这个</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G5" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <rFont val="宋体"/>
-            <charset val="134"/>
-          </rPr>
-          <t>list为无主键表</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G6" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <rFont val="宋体"/>
-            <charset val="134"/>
-          </rPr>
-          <t>one为单例表</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>##var</t>
   </si>
@@ -181,46 +110,52 @@
     <t>默认为 &lt;module&gt;_&lt;name&gt;.&lt;suffix&gt;</t>
   </si>
   <si>
-    <t>Examples.TbExampleBasic</t>
-  </si>
-  <si>
-    <t>ExampleBasic</t>
-  </si>
-  <si>
-    <t>../基础@_示例.xlsx</t>
-  </si>
-  <si>
-    <t>Examples.TbExampleAdvance</t>
-  </si>
-  <si>
-    <t>ExampleAdvance</t>
-  </si>
-  <si>
-    <t>../复杂类型@_示例.xlsx</t>
+    <t>Examples.TbBasicConfig</t>
+  </si>
+  <si>
+    <t>BasicConfig</t>
+  </si>
+  <si>
+    <t>TRUE</t>
+  </si>
+  <si>
+    <t>../Examples.BasicConfig@_示例.xlsx</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Examples.TbAdavancedConfig</t>
+  </si>
+  <si>
+    <t>AdavancedConfig</t>
+  </si>
+  <si>
+    <t>../Examples.AdavancedConfig#list@_示例.xlsx</t>
   </si>
   <si>
     <t>list</t>
   </si>
   <si>
-    <t>Examples.TbExampleSingleton</t>
-  </si>
-  <si>
-    <t>ExampleSingleton</t>
-  </si>
-  <si>
-    <t>../纵表@_示例.xlsx</t>
+    <t>Examples.TbGlobalConfig</t>
+  </si>
+  <si>
+    <t>GlobalConfig</t>
+  </si>
+  <si>
+    <t>../Examples.GlobalConfig#one@_示例.xlsx</t>
   </si>
   <si>
     <t>one</t>
   </si>
   <si>
-    <t>Examples.TbExampleList</t>
-  </si>
-  <si>
-    <t>ExampleList</t>
-  </si>
-  <si>
-    <t>../列表表@_示例.xlsx</t>
+    <t>Examples.TbListConfig</t>
+  </si>
+  <si>
+    <t>ListConfig</t>
+  </si>
+  <si>
+    <t>../Examples.ListConfig#list@_示例.xlsx</t>
   </si>
 </sst>
 </file>
@@ -233,7 +168,7 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -247,12 +182,6 @@
       <name val="等线"/>
       <charset val="134"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="微软雅黑"/>
-      <charset val="134"/>
     </font>
     <font>
       <u/>
@@ -390,11 +319,6 @@
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="宋体"/>
-      <charset val="134"/>
     </font>
   </fonts>
   <fills count="33">
@@ -714,165 +638,162 @@
     </border>
   </borders>
   <cellStyleXfs count="49">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" applyNumberFormat="1" fontId="0" applyFont="0" fillId="0" applyFill="0" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" applyNumberFormat="1" fontId="0" applyFont="0" fillId="0" applyFill="0" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" applyNumberFormat="1" fontId="0" applyFont="0" fillId="0" applyFill="0" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" applyNumberFormat="1" fontId="0" applyFont="0" fillId="0" applyFill="0" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" applyNumberFormat="1" fontId="0" applyFont="0" fillId="0" applyFill="0" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="2" applyFont="1" fillId="0" applyFill="0" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="3" applyFont="1" fillId="0" applyFill="0" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="0" applyFont="0" fillId="3" applyFill="1" borderId="2" applyBorder="1" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="4" applyFont="1" fillId="0" applyFill="0" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="5" applyFont="1" fillId="0" applyFill="0" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="6" applyFont="1" fillId="0" applyFill="0" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="7" applyFont="1" fillId="0" applyFill="0" borderId="3" applyBorder="1" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="8" applyFont="1" fillId="0" applyFill="0" borderId="3" applyBorder="1" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="9" applyFont="1" fillId="0" applyFill="0" borderId="4" applyBorder="1" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="9" applyFont="1" fillId="0" applyFill="0" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="10" applyFont="1" fillId="4" applyFill="1" borderId="5" applyBorder="1" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="11" applyFont="1" fillId="5" applyFill="1" borderId="6" applyBorder="1" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="12" applyFont="1" fillId="5" applyFill="1" borderId="5" applyBorder="1" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="13" applyFont="1" fillId="6" applyFill="1" borderId="7" applyBorder="1" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="14" applyFont="1" fillId="0" applyFill="0" borderId="8" applyBorder="1" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="15" applyFont="1" fillId="0" applyFill="0" borderId="9" applyBorder="1" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="1" applyFont="1" fillId="2" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="16" applyFont="1" fillId="7" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="17" applyFont="1" fillId="8" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="18" applyFont="1" fillId="9" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="19" applyFont="1" fillId="10" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="19" applyFont="1" fillId="11" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="18" applyFont="1" fillId="12" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="18" applyFont="1" fillId="13" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="19" applyFont="1" fillId="14" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="19" applyFont="1" fillId="15" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="18" applyFont="1" fillId="16" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="18" applyFont="1" fillId="17" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="19" applyFont="1" fillId="18" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="19" applyFont="1" fillId="19" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="18" applyFont="1" fillId="20" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="18" applyFont="1" fillId="21" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="19" applyFont="1" fillId="22" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="19" applyFont="1" fillId="23" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="18" applyFont="1" fillId="24" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="18" applyFont="1" fillId="25" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="19" applyFont="1" fillId="26" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="19" applyFont="1" fillId="27" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="18" applyFont="1" fillId="28" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="18" applyFont="1" fillId="29" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="19" applyFont="1" fillId="30" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="19" applyFont="1" fillId="31" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="18" applyFont="1" fillId="32" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="22">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="22" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" applyFont="1" fillId="2" applyFill="1" borderId="0" xfId="22" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" applyFont="1" fillId="2" applyFill="1" borderId="1" applyBorder="1" xfId="22" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1194,13 +1115,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:K22"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" outlineLevelRow="6"/>
   <cols>
     <col min="2" max="2" width="36.4444444444444" customWidth="1"/>
     <col min="3" max="3" width="29.3333333333333" customWidth="1"/>
@@ -1209,7 +1130,7 @@
     <col min="6" max="9" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:11">
+    <row r="1" s="1" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1244,7 +1165,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" s="1" customFormat="1" spans="1:11">
+    <row r="2" s="1" customFormat="1">
       <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
@@ -1277,7 +1198,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" s="1" customFormat="1" spans="1:11">
+    <row r="3" s="1" customFormat="1">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
@@ -1304,219 +1225,77 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" ht="15.6" spans="2:7">
-      <c r="B4" s="3" t="s">
+    <row r="4">
+      <c r="B4" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E4" s="3" t="s">
+      <c r="D4" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
+      <c r="E4" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="5" ht="15.6" spans="2:7">
-      <c r="B5" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E5" s="3" t="s">
+    <row r="5">
+      <c r="B5" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3" t="s">
+      <c r="C5" s="0" t="s">
         <v>33</v>
       </c>
+      <c r="D5" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="6" ht="15.6" spans="2:9">
-      <c r="B6" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6" s="3" t="s">
+    <row r="6">
+      <c r="B6" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="G7" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-    </row>
-    <row r="7" ht="15.6" spans="2:9">
-      <c r="B7" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D7" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-    </row>
-    <row r="8" ht="15.6" spans="3:9">
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-    </row>
-    <row r="9" ht="15.6" spans="3:9">
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-    </row>
-    <row r="10" ht="15.6" spans="3:9">
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-    </row>
-    <row r="11" ht="15.6" spans="3:9">
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-    </row>
-    <row r="12" ht="15.6" spans="3:9">
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-    </row>
-    <row r="13" ht="15.6" spans="3:9">
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-    </row>
-    <row r="14" ht="15.6" spans="3:9">
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-    </row>
-    <row r="15" ht="15.6" spans="3:9">
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-    </row>
-    <row r="16" ht="15.6" spans="3:9">
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-    </row>
-    <row r="17" ht="15.6" spans="3:9">
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-    </row>
-    <row r="18" ht="15.6" spans="3:9">
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-    </row>
-    <row r="19" ht="15.6" spans="3:9">
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-    </row>
-    <row r="20" ht="15.6" spans="3:9">
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-    </row>
-    <row r="21" ht="15.6" spans="3:9">
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-    </row>
-    <row r="22" ht="15.6" spans="3:9">
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>